<commit_message>
Adecuacion Centralizador Calificaciones RM 0189/2023
</commit_message>
<xml_diff>
--- a/web/resources/uploads/centralizador.xlsx
+++ b/web/resources/uploads/centralizador.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t xml:space="preserve">Código de Registro: </t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;&lt;CONDICION&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;*&gt;&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">JEFE(A) DE CARRERA </t>
@@ -506,16 +509,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -523,35 +530,35 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -559,31 +566,31 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -591,19 +598,19 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -611,7 +618,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -619,11 +626,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -631,11 +638,11 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -655,11 +662,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -667,43 +674,43 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -784,19 +791,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>60840</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>53280</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>144360</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2229480</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>144360</xdr:rowOff>
+      <xdr:rowOff>66960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="Imagen 2" descr=""/>
+        <xdr:cNvPr id="0" name="Image 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -805,8 +812,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="60840" y="243720"/>
-          <a:ext cx="3294000" cy="1005480"/>
+          <a:off x="0" y="303480"/>
+          <a:ext cx="3200400" cy="868320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -834,436 +841,438 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="5" style="0" width="10.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="5" style="1" width="10.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="K1" s="2" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="K1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="6"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="9"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="7"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="10" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="11" t="s">
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="11"/>
-      <c r="P4" s="12" t="n">
+      <c r="O4" s="12"/>
+      <c r="P4" s="13" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="11" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="11"/>
-      <c r="P5" s="12" t="n">
+      <c r="O5" s="12"/>
+      <c r="P5" s="13" t="n">
         <v>-2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="15"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="16"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="N7" s="2" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="N7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="O7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="3"/>
+      <c r="P7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="21" t="s">
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="J8" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="20"/>
-      <c r="N8" s="22" t="s">
+      <c r="K8" s="21"/>
+      <c r="N8" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="O8" s="20" t="s">
+      <c r="O8" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="P8" s="23"/>
+      <c r="P8" s="24"/>
     </row>
     <row r="9" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="25" t="s">
+      <c r="B9" s="25"/>
+      <c r="C9" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="27" t="s">
+      <c r="H9" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="27" t="s">
+      <c r="J9" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="K9" s="27" t="s">
+      <c r="K9" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="L9" s="27" t="s">
+      <c r="L9" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="M9" s="27" t="s">
+      <c r="M9" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="27" t="s">
+      <c r="N9" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="O9" s="28" t="s">
+      <c r="O9" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="P9" s="28"/>
+      <c r="P9" s="29"/>
     </row>
     <row r="10" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="25" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="30" t="s">
+      <c r="D10" s="27"/>
+      <c r="E10" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="30" t="s">
+      <c r="F10" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="H10" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="I10" s="30" t="s">
+      <c r="I10" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="30" t="s">
+      <c r="J10" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="K10" s="30" t="s">
+      <c r="K10" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="L10" s="30" t="s">
+      <c r="L10" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="M10" s="30" t="s">
+      <c r="M10" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="N10" s="30" t="s">
+      <c r="N10" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="O10" s="28"/>
-      <c r="P10" s="28"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
     </row>
     <row r="11" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="25" t="s">
+      <c r="B11" s="25"/>
+      <c r="C11" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
     </row>
     <row r="12" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25" t="s">
+      <c r="B12" s="25"/>
+      <c r="C12" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
     </row>
     <row r="13" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="25" t="s">
+      <c r="B13" s="25"/>
+      <c r="C13" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="32" t="n">
+      <c r="A15" s="33" t="n">
         <v>-3</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="34" t="s">
+      <c r="C15" s="34"/>
+      <c r="D15" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="35" t="n">
+      <c r="E15" s="36" t="n">
         <v>-10</v>
       </c>
-      <c r="F15" s="35" t="n">
+      <c r="F15" s="36" t="n">
         <v>-20</v>
       </c>
-      <c r="G15" s="35" t="n">
+      <c r="G15" s="36" t="n">
         <v>-30</v>
       </c>
-      <c r="H15" s="35" t="n">
+      <c r="H15" s="36" t="n">
         <v>-40</v>
       </c>
-      <c r="I15" s="35" t="n">
+      <c r="I15" s="36" t="n">
         <v>-50</v>
       </c>
-      <c r="J15" s="35" t="n">
+      <c r="J15" s="36" t="n">
         <v>-60</v>
       </c>
-      <c r="K15" s="35" t="n">
+      <c r="K15" s="36" t="n">
         <v>-70</v>
       </c>
-      <c r="L15" s="35" t="n">
+      <c r="L15" s="36" t="n">
         <v>-80</v>
       </c>
-      <c r="M15" s="35" t="n">
+      <c r="M15" s="36" t="n">
         <v>-90</v>
       </c>
-      <c r="N15" s="35" t="n">
+      <c r="N15" s="36" t="n">
         <v>-100</v>
       </c>
-      <c r="O15" s="36" t="s">
+      <c r="O15" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="P15" s="36"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="37"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
+      <c r="P15" s="37"/>
+    </row>
+    <row r="16" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="40"/>
+      <c r="P16" s="40"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="37"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="38"/>
-      <c r="P17" s="38"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="39"/>
+      <c r="P17" s="39"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C20" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" s="40" t="s">
+      <c r="C20" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="J20" s="40" t="s">
+      <c r="E20" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
-      <c r="N20" s="41" t="s">
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="J20" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="O20" s="41"/>
-      <c r="P20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="N20" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="O20" s="42"/>
+      <c r="P20" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="34">
     <mergeCell ref="M1:P1"/>
     <mergeCell ref="A2:C6"/>
     <mergeCell ref="D4:M6"/>
@@ -1295,7 +1304,6 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="O15:P15"/>
-    <mergeCell ref="K16:P16"/>
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="J20:L20"/>
     <mergeCell ref="N20:P20"/>
@@ -1319,129 +1327,129 @@
   <dimension ref="B19:T25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q25" activeCellId="0" sqref="Q25"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.67"/>
   </cols>
   <sheetData>
     <row r="19" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E19" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
+      <c r="E19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M20" s="42"/>
-      <c r="N20" s="42"/>
-      <c r="O20" s="42"/>
-      <c r="P20" s="42"/>
-      <c r="Q20" s="42"/>
-      <c r="R20" s="42"/>
-      <c r="S20" s="42"/>
-      <c r="T20" s="42"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="43"/>
+      <c r="P20" s="43"/>
+      <c r="Q20" s="43"/>
+      <c r="R20" s="43"/>
+      <c r="S20" s="43"/>
+      <c r="T20" s="43"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="44" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44" t="s">
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="K21" s="44" t="s">
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="M21" s="45"/>
+      <c r="K21" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="M21" s="46"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="46"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="48" t="n">
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="49" t="n">
         <v>-10</v>
       </c>
-      <c r="K22" s="49" t="n">
+      <c r="K22" s="50" t="n">
         <v>-0.2</v>
       </c>
-      <c r="M22" s="45"/>
+      <c r="M22" s="46"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="48" t="n">
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="48"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="49" t="n">
         <v>-30</v>
       </c>
-      <c r="K23" s="49" t="n">
+      <c r="K23" s="50" t="n">
         <v>-0.4</v>
       </c>
-      <c r="M23" s="45"/>
+      <c r="M23" s="46"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="46"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="48" t="n">
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="49" t="n">
         <v>-50</v>
       </c>
-      <c r="K24" s="49" t="n">
+      <c r="K24" s="50" t="n">
         <v>-0.6</v>
       </c>
-      <c r="M24" s="45"/>
+      <c r="M24" s="46"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="46"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="F25" s="47"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47"/>
-      <c r="I25" s="47"/>
-      <c r="J25" s="48" t="n">
+      <c r="B25" s="47"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="49" t="n">
         <v>-70</v>
       </c>
-      <c r="K25" s="49" t="n">
+      <c r="K25" s="50" t="n">
         <v>-0.8</v>
       </c>
-      <c r="M25" s="45"/>
+      <c r="M25" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Adecuacion Centralizador de Calificaciones DDE/SESFP/INS/0146/2024
</commit_message>
<xml_diff>
--- a/web/resources/uploads/centralizador.xlsx
+++ b/web/resources/uploads/centralizador.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="91">
   <si>
     <t xml:space="preserve">Código de Registro: </t>
   </si>
@@ -124,6 +124,9 @@
     <t xml:space="preserve">&lt;&lt;C10&gt;&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">ESTADO</t>
+  </si>
+  <si>
     <t xml:space="preserve">OBSERVACIONES </t>
   </si>
   <si>
@@ -187,15 +190,51 @@
     <t xml:space="preserve">NÓMINA ESTUDIANTES</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;&lt;N&gt;&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;&lt;ESTUDIANTE&gt;&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;&lt;CI&gt;&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;&lt;A&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;B&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;C&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;D&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;E&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;F&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;G&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;H&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;I&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;J&gt;&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;&lt;CONDICION&gt;&gt;</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;&lt;OBSERVACION&gt;&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;&lt;*&gt;&gt;</t>
   </si>
   <si>
@@ -211,6 +250,48 @@
     <t xml:space="preserve">SELLO S.E.S.</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;&lt;D1&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;D2&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;D3&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;D4&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;D5&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;D6&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;D7&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;D8&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;D9&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;D10&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;D11&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;D12&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;M11&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&lt;M12&gt;&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">ESTADISTICAS</t>
   </si>
   <si>
@@ -232,7 +313,7 @@
     <t xml:space="preserve">ESTUDIANTES REPROBADOS</t>
   </si>
   <si>
-    <t xml:space="preserve">NO SE PRESENTARON</t>
+    <t xml:space="preserve">ABANDONO</t>
   </si>
 </sst>
 </file>
@@ -336,6 +417,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
@@ -343,20 +431,19 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -509,7 +596,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -530,6 +617,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -578,7 +669,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -618,15 +709,19 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -634,11 +729,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -646,11 +737,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -682,6 +773,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -690,16 +785,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -797,9 +892,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2229480</xdr:colOff>
+      <xdr:colOff>1989720</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>66960</xdr:rowOff>
+      <xdr:rowOff>80640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -813,7 +908,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="303480"/>
-          <a:ext cx="3200400" cy="868320"/>
+          <a:ext cx="3361320" cy="865440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -828,24 +923,132 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.68359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="5" style="1" width="10.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="5" style="1" width="10.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="14.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="16.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -855,389 +1058,406 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
-      <c r="K1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4"/>
+      <c r="P1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-    </row>
-    <row r="2" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="7"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="9"/>
+      <c r="Q1" s="5"/>
+    </row>
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="8"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="10"/>
       <c r="P3" s="10"/>
+      <c r="Q3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="11" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="12" t="s">
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="12"/>
-      <c r="P4" s="13" t="n">
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="14" t="n">
         <v>-1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="12" t="s">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="12"/>
-      <c r="P5" s="13" t="n">
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="14" t="n">
         <v>-2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="15"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="16"/>
       <c r="P6" s="16"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
+      <c r="Q6" s="17"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="18"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="19"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
       <c r="N7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="O7" s="3"/>
+      <c r="P7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="4"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20" t="s">
+      <c r="Q7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="21" t="s">
+      <c r="B8" s="21"/>
+      <c r="C8" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="22" t="s">
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="21"/>
-      <c r="N8" s="23" t="s">
+      <c r="K8" s="22"/>
+      <c r="N8" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="O8" s="21" t="s">
+      <c r="O8" s="24"/>
+      <c r="P8" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="P8" s="24"/>
+      <c r="Q8" s="25"/>
     </row>
     <row r="9" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="26" t="s">
+      <c r="B9" s="26"/>
+      <c r="C9" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="28" t="s">
+      <c r="H9" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="28" t="s">
+      <c r="I9" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="28" t="s">
+      <c r="J9" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="K9" s="28" t="s">
+      <c r="K9" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="L9" s="28" t="s">
+      <c r="L9" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="M9" s="28" t="s">
+      <c r="M9" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="28" t="s">
+      <c r="N9" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="O9" s="29" t="s">
+      <c r="O9" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="P9" s="29"/>
+      <c r="P9" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q9" s="31"/>
     </row>
     <row r="10" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="26" t="s">
+      <c r="A10" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="31" t="s">
+      <c r="B10" s="32"/>
+      <c r="C10" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="31" t="s">
+      <c r="D10" s="28"/>
+      <c r="E10" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="31" t="s">
+      <c r="F10" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="G10" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="I10" s="31" t="s">
+      <c r="H10" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="J10" s="31" t="s">
+      <c r="I10" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="K10" s="31" t="s">
+      <c r="J10" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="L10" s="31" t="s">
+      <c r="K10" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="M10" s="31" t="s">
+      <c r="L10" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="N10" s="31" t="s">
+      <c r="M10" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
+      <c r="N10" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="O10" s="30"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
     </row>
     <row r="11" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="26" t="s">
+      <c r="A11" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="27"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
     </row>
     <row r="12" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="26" t="s">
+      <c r="A12" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="27"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="28"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
     </row>
     <row r="13" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="26" t="s">
+      <c r="A13" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="32" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="D13" s="28"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31"/>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="33" t="n">
-        <v>-3</v>
-      </c>
-      <c r="B15" s="34" t="s">
+      <c r="B14" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="35" t="s">
+      <c r="C14" s="33"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="31"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="36" t="n">
-        <v>-10</v>
-      </c>
-      <c r="F15" s="36" t="n">
-        <v>-20</v>
-      </c>
-      <c r="G15" s="36" t="n">
-        <v>-30</v>
-      </c>
-      <c r="H15" s="36" t="n">
-        <v>-40</v>
-      </c>
-      <c r="I15" s="36" t="n">
-        <v>-50</v>
-      </c>
-      <c r="J15" s="36" t="n">
-        <v>-60</v>
-      </c>
-      <c r="K15" s="36" t="n">
-        <v>-70</v>
-      </c>
-      <c r="L15" s="36" t="n">
-        <v>-80</v>
-      </c>
-      <c r="M15" s="36" t="n">
-        <v>-90</v>
-      </c>
-      <c r="N15" s="36" t="n">
-        <v>-100</v>
+      <c r="B15" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="35"/>
+      <c r="D15" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="J15" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="K15" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="L15" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="M15" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="N15" s="37" t="s">
+        <v>61</v>
       </c>
       <c r="O15" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="P15" s="37"/>
+        <v>62</v>
+      </c>
+      <c r="P15" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q15" s="38"/>
     </row>
     <row r="16" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
+      <c r="A16" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="40"/>
-      <c r="N16" s="40"/>
-      <c r="O16" s="40"/>
-      <c r="P16" s="40"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K16" s="41"/>
+      <c r="L16" s="41"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="41"/>
+      <c r="Q16" s="41"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1248,45 +1468,48 @@
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="40"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C20" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="J20" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="N20" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="O20" s="42"/>
-      <c r="P20" s="42"/>
+      <c r="C20" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="J20" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="N20" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="O20" s="43"/>
+      <c r="P20" s="43"/>
+      <c r="Q20" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="M1:P1"/>
+  <mergeCells count="35">
+    <mergeCell ref="P1:Q1"/>
     <mergeCell ref="A2:C6"/>
     <mergeCell ref="D4:M6"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N5:P5"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="J7:K7"/>
-    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="P7:Q7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:H8"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="D9:D14"/>
-    <mergeCell ref="O9:P14"/>
+    <mergeCell ref="O9:O14"/>
+    <mergeCell ref="P9:Q14"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="E10:E14"/>
     <mergeCell ref="F10:F14"/>
@@ -1303,10 +1526,10 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="P15:Q15"/>
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="J20:L20"/>
-    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="N20:Q20"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1324,141 +1547,313 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="B19:T25"/>
+  <dimension ref="B9:T39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.68359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="1" style="1" width="12.32"/>
   </cols>
   <sheetData>
-    <row r="19" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E19" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="O9" s="44"/>
+      <c r="P9" s="44"/>
+      <c r="Q9" s="44"/>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="44"/>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="K19" s="44"/>
+      <c r="L19" s="44"/>
+      <c r="M19" s="44"/>
+      <c r="N19" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="O19" s="44"/>
+      <c r="P19" s="44"/>
+      <c r="Q19" s="44"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M20" s="43"/>
-      <c r="N20" s="43"/>
-      <c r="O20" s="43"/>
-      <c r="P20" s="43"/>
-      <c r="Q20" s="43"/>
-      <c r="R20" s="43"/>
-      <c r="S20" s="43"/>
-      <c r="T20" s="43"/>
+      <c r="B20" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="K20" s="44"/>
+      <c r="L20" s="44"/>
+      <c r="M20" s="44"/>
+      <c r="N20" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="O20" s="44"/>
+      <c r="P20" s="44"/>
+      <c r="Q20" s="44"/>
+      <c r="R20" s="45"/>
+      <c r="S20" s="45"/>
+      <c r="T20" s="45"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="44"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="K21" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="M21" s="46"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="M21" s="47"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="47"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="48"/>
-      <c r="J22" s="49" t="n">
+      <c r="B22" s="48"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="48"/>
+      <c r="M22" s="47"/>
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B23" s="48"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="48"/>
+      <c r="M23" s="47"/>
+    </row>
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="48"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="M24" s="47"/>
+    </row>
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
+      <c r="M25" s="47"/>
+    </row>
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="K29" s="44"/>
+      <c r="L29" s="44"/>
+      <c r="M29" s="44"/>
+      <c r="N29" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="O29" s="44"/>
+      <c r="P29" s="44"/>
+      <c r="Q29" s="44"/>
+    </row>
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="K30" s="44"/>
+      <c r="L30" s="44"/>
+      <c r="M30" s="44"/>
+      <c r="N30" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="O30" s="44"/>
+      <c r="P30" s="44"/>
+      <c r="Q30" s="44"/>
+    </row>
+    <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G33" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+    </row>
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G35" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="49" t="s">
+        <v>85</v>
+      </c>
+      <c r="K35" s="49" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G36" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="H36" s="50"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="51" t="n">
         <v>-10</v>
       </c>
-      <c r="K22" s="50" t="n">
+      <c r="K36" s="52" t="n">
         <v>-0.2</v>
       </c>
-      <c r="M22" s="46"/>
-    </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="49" t="n">
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G37" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="H37" s="50"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="51" t="n">
         <v>-30</v>
       </c>
-      <c r="K23" s="50" t="n">
+      <c r="K37" s="52" t="n">
         <v>-0.4</v>
       </c>
-      <c r="M23" s="46"/>
-    </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="49" t="n">
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G38" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="H38" s="50"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="51" t="n">
         <v>-50</v>
       </c>
-      <c r="K24" s="50" t="n">
+      <c r="K38" s="52" t="n">
         <v>-0.6</v>
       </c>
-      <c r="M24" s="46"/>
-    </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="47"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="48" t="s">
-        <v>63</v>
-      </c>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="49" t="n">
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G39" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="H39" s="50"/>
+      <c r="I39" s="50"/>
+      <c r="J39" s="51" t="n">
         <v>-70</v>
       </c>
-      <c r="K25" s="50" t="n">
+      <c r="K39" s="52" t="n">
         <v>-0.8</v>
       </c>
-      <c r="M25" s="46"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="E19:K19"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E25:I25"/>
+  <mergeCells count="30">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="N10:Q10"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="N19:Q19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="J20:M20"/>
+    <mergeCell ref="N20:Q20"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="N29:Q29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="J30:M30"/>
+    <mergeCell ref="N30:Q30"/>
+    <mergeCell ref="G33:K33"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="G39:I39"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Fix: Plantilla Excel Centralizador de Calificaciones DDE/SESFP/INS/0146/2024
</commit_message>
<xml_diff>
--- a/web/resources/uploads/centralizador.xlsx
+++ b/web/resources/uploads/centralizador.xlsx
@@ -754,7 +754,7 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -892,9 +892,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1989720</xdr:colOff>
+      <xdr:colOff>1988640</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>80640</xdr:rowOff>
+      <xdr:rowOff>79560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -908,7 +908,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="303480"/>
-          <a:ext cx="3361320" cy="865440"/>
+          <a:ext cx="3360240" cy="864360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1048,6 +1048,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="5" style="1" width="10.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="14.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="16.53"/>
   </cols>
   <sheetData>
@@ -1432,12 +1433,12 @@
       </c>
       <c r="Q15" s="38"/>
     </row>
-    <row r="16" customFormat="false" ht="23.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
       <c r="D16" s="40"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -1494,7 +1495,7 @@
       <c r="Q20" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="36">
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="A2:C6"/>
     <mergeCell ref="D4:M6"/>
@@ -1527,6 +1528,7 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="A16:C16"/>
     <mergeCell ref="E20:G20"/>
     <mergeCell ref="J20:L20"/>
     <mergeCell ref="N20:Q20"/>

</xml_diff>